<commit_message>
added comparison with the previous period plot
</commit_message>
<xml_diff>
--- a/data/daily_donations_by_category.xlsx
+++ b/data/daily_donations_by_category.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,19 +446,19 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Victory Drones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>1000 Drones for Ukraine</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Mobile Shower Units</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Victory Drones</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Flight to Recovery</t>
@@ -471,46 +471,70 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Veteranius</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>grants</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Admin</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>bank fees &amp; service charges</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-05-03</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6612.99</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>1869.67</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>131.57</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>87.22</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>2023-05-05</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1292.32</v>
+        <v>175</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -519,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>102.53</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -528,45 +552,63 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-05-10</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1316.35</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>1240.29</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>880.05</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>103.48</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>155.47</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-05-18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>207.57</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -581,20 +623,29 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>51.52</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-05-20</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>98.43000000000001</v>
+        <v>270</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -612,23 +663,32 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-05-21</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1115.65</v>
+        <v>425</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -640,20 +700,29 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-05-22</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>51.52</v>
+        <v>1711</v>
       </c>
       <c r="C8" t="n">
-        <v>204.56</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -668,23 +737,32 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>2023-05-27</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>339.5</v>
+        <v>360</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -696,23 +774,32 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>2023-05-29</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>204.13</v>
+        <v>0.97</v>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -724,17 +811,26 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>2023-05-30</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>87.99000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -752,48 +848,66 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2023-05-31</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2251</v>
+        <v>230.54</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>510.65</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>51.52</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-11-14</t>
+          <t>2023-06-03</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10.7</v>
+        <v>40</v>
       </c>
       <c r="C13" t="n">
-        <v>10.7</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -808,17 +922,26 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-11-15</t>
+          <t>2023-06-05</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>388.72</v>
+        <v>5.64</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -836,17 +959,26 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-11-16</t>
+          <t>2023-06-06</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>246.61</v>
+        <v>637</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -864,26 +996,35 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-11-17</t>
+          <t>2023-06-07</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>65.8</v>
+        <v>100</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>760</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>3.59</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -892,23 +1033,32 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-11-18</t>
+          <t>2023-06-10</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>398</v>
+        <v>170</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -920,20 +1070,29 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-11-19</t>
+          <t>2023-06-14</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>101.83</v>
+        <v>98</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -948,20 +1107,29 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2023-06-17</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>295.33</v>
+        <v>185</v>
       </c>
       <c r="C19" t="n">
-        <v>57.12</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -976,17 +1144,26 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-11-21</t>
+          <t>2023-06-18</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>139.44</v>
+        <v>200</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -1001,23 +1178,32 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>255.58</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-11-22</t>
+          <t>2023-06-23</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>541.75</v>
+        <v>80</v>
       </c>
       <c r="C21" t="n">
-        <v>173.75</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1032,17 +1218,26 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-11-23</t>
+          <t>2023-06-24</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>726.28</v>
+        <v>540</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -1051,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>103.59</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1060,20 +1255,29 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-11-25</t>
+          <t>2023-06-26</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>185.14</v>
+        <v>58.75</v>
       </c>
       <c r="C23" t="n">
-        <v>868.76</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1088,23 +1292,32 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-11-26</t>
+          <t>2023-06-30</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>234.56</v>
+        <v>60</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1116,45 +1329,63 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-07-01</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1459.53</v>
+        <v>117.2</v>
       </c>
       <c r="C25" t="n">
-        <v>155.53</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>103.48</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>26.25</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2023-11-30</t>
+          <t>2023-07-08</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17.56</v>
+        <v>750</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -1172,34 +1403,2309 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>2023-07-15</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>130</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-07-18</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>141.85</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>146.95</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>40</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-07-27</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>633.13</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-07-30</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-08-10</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>100</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-08-11</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>30</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-08-19</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>120</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>300</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-08-26</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>60</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2023-08-27</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1010</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-08-28</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2100</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-08-30</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2400</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>565</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-09-02</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2023-09-06</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>500</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2023-09-09</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>110</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2023-09-10</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2023-09-14</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>739.96</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2023-09-16</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>25</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2023-09-17</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>140</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2023-09-21</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>30</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2023-09-22</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>41858.94</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1578.54</v>
+      </c>
+      <c r="D51" t="n">
+        <v>6288.62</v>
+      </c>
+      <c r="E51" t="n">
+        <v>596.4100000000001</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-09-23</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>29354.79</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1623.76</v>
+      </c>
+      <c r="D52" t="n">
+        <v>6209.72</v>
+      </c>
+      <c r="E52" t="n">
+        <v>253.98</v>
+      </c>
+      <c r="F52" t="n">
+        <v>693.46</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>155.55</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-09-24</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>306.59</v>
+      </c>
+      <c r="C53" t="n">
+        <v>102.53</v>
+      </c>
+      <c r="D53" t="n">
+        <v>610.65</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>51.52</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>31.11</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>245</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-09-26</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-09-27</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2023-10-04</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>218.32</v>
+      </c>
+      <c r="C57" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2023-10-05</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>25</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1281.27</v>
+      </c>
+      <c r="C59" t="n">
+        <v>180</v>
+      </c>
+      <c r="D59" t="n">
+        <v>413.55</v>
+      </c>
+      <c r="E59" t="n">
+        <v>20.91</v>
+      </c>
+      <c r="F59" t="n">
+        <v>176.38</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>164.56</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2023-10-15</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>100</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2023-10-19</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>522.5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2023-11-02</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6612.99</v>
+      </c>
+      <c r="C63" t="n">
+        <v>131.57</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1869.67</v>
+      </c>
+      <c r="E63" t="n">
+        <v>25</v>
+      </c>
+      <c r="F63" t="n">
+        <v>87.22</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2023-11-03</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1292.32</v>
+      </c>
+      <c r="C64" t="n">
+        <v>102.53</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2023-11-05</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1316.35</v>
+      </c>
+      <c r="C65" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1240.29</v>
+      </c>
+      <c r="E65" t="n">
+        <v>880.05</v>
+      </c>
+      <c r="F65" t="n">
+        <v>155.47</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>207.57</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>51.52</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2023-11-07</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>98.43000000000001</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2023-11-08</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1115.65</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>50</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>51.52</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>204.56</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-11-10</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>339.5</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>360</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-11-11</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>204.13</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>100</v>
+      </c>
+      <c r="E71" t="n">
+        <v>400</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-11-12</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>87.99000000000001</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>2251</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>510.65</v>
+      </c>
+      <c r="F73" t="n">
+        <v>51.52</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-11-14</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-11-15</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>388.72</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-11-16</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>246.61</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-11-17</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="C77" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>760</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-11-18</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>398</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>50</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-11-19</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>101.83</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>20</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>295.33</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>57.12</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-11-21</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>139.44</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>255.58</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2023-11-22</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>541.75</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>173.75</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2023-11-23</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>726.28</v>
+      </c>
+      <c r="C83" t="n">
+        <v>103.59</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-11-25</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>185.14</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>868.76</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2023-11-26</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>234.56</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>100</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1459.53</v>
+      </c>
+      <c r="C86" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="D86" t="n">
+        <v>155.53</v>
+      </c>
+      <c r="E86" t="n">
+        <v>50</v>
+      </c>
+      <c r="F86" t="n">
+        <v>20</v>
+      </c>
+      <c r="G86" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-09-28</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>100</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>2023-11-24</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="n">
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
         <v>26.01</v>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
         <v>51.52</v>
       </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" t="n">
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data upd and area plot for cumulative donations added
</commit_message>
<xml_diff>
--- a/data/daily_donations_by_category.xlsx
+++ b/data/daily_donations_by_category.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2865,7 +2865,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>207.57</v>
+        <v>259.09</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -2880,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>51.52</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -3638,20 +3638,20 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2023-09-28</t>
+          <t>2023-11-28</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>270.57</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>100</v>
+        <v>102.53</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -3675,37 +3675,481 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>2023-11-29</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="C88" t="n">
+        <v>50</v>
+      </c>
+      <c r="D88" t="n">
+        <v>224.45</v>
+      </c>
+      <c r="E88" t="n">
+        <v>45</v>
+      </c>
+      <c r="F88" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-11-30</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>432.11</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>144.35</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>77.77000000000001</v>
+      </c>
+      <c r="E90" t="n">
+        <v>600</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-12-02</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>437.15</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>46.83</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2023-12-03</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>41.31</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>73.90000000000001</v>
+      </c>
+      <c r="C93" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="D93" t="n">
+        <v>200</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>103.48</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2023-12-05</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>122.53</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>50</v>
+      </c>
+      <c r="E94" t="n">
+        <v>141</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023-12-06</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>76.52000000000001</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>404.56</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-12-07</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>630.76</v>
+      </c>
+      <c r="C96" t="n">
+        <v>113.23</v>
+      </c>
+      <c r="D96" t="n">
+        <v>35</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-12-08</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>71.52000000000001</v>
+      </c>
+      <c r="C97" t="n">
+        <v>307.09</v>
+      </c>
+      <c r="D97" t="n">
+        <v>300</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023-12-09</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1204.56</v>
+      </c>
+      <c r="C98" t="n">
+        <v>77.02</v>
+      </c>
+      <c r="D98" t="n">
+        <v>51.52</v>
+      </c>
+      <c r="E98" t="n">
+        <v>510</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2023-09-28</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>100</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
           <t>2023-11-24</t>
         </is>
       </c>
-      <c r="B88" t="n">
-        <v>0</v>
-      </c>
-      <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="n">
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
         <v>26.01</v>
       </c>
-      <c r="E88" t="n">
-        <v>0</v>
-      </c>
-      <c r="F88" t="n">
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
         <v>51.52</v>
       </c>
-      <c r="G88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H88" t="n">
-        <v>0</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" t="n">
-        <v>0</v>
-      </c>
-      <c r="K88" t="n">
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>